<commit_message>
fixing texts in pricing section
</commit_message>
<xml_diff>
--- a/assets/texts/pricing/pricing.xlsx
+++ b/assets/texts/pricing/pricing.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hareltussi/Desktop/work/dpl-next/assets/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hareltussi/Desktop/work/dpl-next/assets/texts/pricing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73555A10-4084-8740-9A5C-4B8B829343BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{183A4F62-191A-2F4D-B3A7-668465961640}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="19200" windowHeight="21700" xr2:uid="{27E80618-E5B8-C54A-AD74-13243F9E4A36}"/>
   </bookViews>
@@ -96,9 +96,6 @@
     <t>Set instant alerts on specific diamonds in a specific price range.</t>
   </si>
   <si>
-    <t>Trusted by Leading Industry Professionals</t>
-  </si>
-  <si>
     <t>thirdSectionHeader</t>
   </si>
   <si>
@@ -195,13 +192,16 @@
     <t>Monthly</t>
   </si>
   <si>
-    <t>Lifetime</t>
-  </si>
-  <si>
     <t>secondSectionHeader1</t>
   </si>
   <si>
     <t>Working with DPL</t>
+  </si>
+  <si>
+    <t>Acknowledged by the industry’s leading professionals</t>
+  </si>
+  <si>
+    <t>Yearly</t>
   </si>
 </sst>
 </file>
@@ -563,7 +563,7 @@
   <dimension ref="A1:B28"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -590,18 +590,18 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
@@ -638,7 +638,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>12</v>
@@ -662,7 +662,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>18</v>
@@ -678,122 +678,122 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>20</v>
+        <v>54</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
+        <v>21</v>
+      </c>
+      <c r="B15" s="1" t="s">
         <v>22</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>

</xml_diff>